<commit_message>
remove catch sheets from main Tyee file
</commit_message>
<xml_diff>
--- a/data/tyee FN catch 2024.xlsx
+++ b/data/tyee FN catch 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29198B15-BF81-8043-971D-0075649BDA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91671601-6ECB-0D46-B14E-AB8D1443C034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8500" yWindow="500" windowWidth="25980" windowHeight="14940" activeTab="2" xr2:uid="{21FFAA14-1E58-C441-A0E9-3C24218A8304}"/>
+    <workbookView xWindow="2820" yWindow="500" windowWidth="25980" windowHeight="14940" xr2:uid="{21FFAA14-1E58-C441-A0E9-3C24218A8304}"/>
   </bookViews>
   <sheets>
     <sheet name="Sockeye FSC and Demo" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -194,9 +194,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -214,6 +211,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -239,16 +239,12 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Stat weeks"/>
-      <sheetName val="Sockeye FSC and Demo"/>
-      <sheetName val="inriver catch"/>
       <sheetName val="Tyee"/>
       <sheetName val="tyee daily"/>
       <sheetName val="tyee cum"/>
       <sheetName val="tyee pcum"/>
       <sheetName val="index"/>
-      <sheetName val="gncatch"/>
       <sheetName val="Sheet1"/>
-      <sheetName val="demo catches"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -1205,199 +1201,12 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
-        <row r="5">
-          <cell r="S5">
-            <v>24</v>
-          </cell>
-          <cell r="T5">
-            <v>0</v>
-          </cell>
-          <cell r="U5">
-            <v>0</v>
-          </cell>
-          <cell r="V5">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="S6">
-            <v>25</v>
-          </cell>
-          <cell r="T6">
-            <v>0</v>
-          </cell>
-          <cell r="U6">
-            <v>0</v>
-          </cell>
-          <cell r="V6">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="S7">
-            <v>26</v>
-          </cell>
-          <cell r="T7">
-            <v>0</v>
-          </cell>
-          <cell r="U7">
-            <v>0</v>
-          </cell>
-          <cell r="V7">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="S8">
-            <v>27</v>
-          </cell>
-          <cell r="T8">
-            <v>0</v>
-          </cell>
-          <cell r="U8">
-            <v>0</v>
-          </cell>
-          <cell r="V8">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="S9">
-            <v>28</v>
-          </cell>
-          <cell r="T9">
-            <v>0</v>
-          </cell>
-          <cell r="U9">
-            <v>2000</v>
-          </cell>
-          <cell r="V9">
-            <v>2000</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="S10">
-            <v>29</v>
-          </cell>
-          <cell r="T10">
-            <v>0</v>
-          </cell>
-          <cell r="U10">
-            <v>7000</v>
-          </cell>
-          <cell r="V10">
-            <v>7000</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="S11">
-            <v>30</v>
-          </cell>
-          <cell r="T11">
-            <v>0</v>
-          </cell>
-          <cell r="U11">
-            <v>12000</v>
-          </cell>
-          <cell r="V11">
-            <v>12000</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="S12">
-            <v>31</v>
-          </cell>
-          <cell r="T12">
-            <v>200</v>
-          </cell>
-          <cell r="U12">
-            <v>17000</v>
-          </cell>
-          <cell r="V12">
-            <v>17200</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="S13">
-            <v>32</v>
-          </cell>
-          <cell r="T13">
-            <v>2000</v>
-          </cell>
-          <cell r="U13">
-            <v>24500</v>
-          </cell>
-          <cell r="V13">
-            <v>26500</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="S14">
-            <v>33</v>
-          </cell>
-          <cell r="T14">
-            <v>6000</v>
-          </cell>
-          <cell r="U14">
-            <v>24500</v>
-          </cell>
-          <cell r="V14">
-            <v>30500</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="S15">
-            <v>34</v>
-          </cell>
-          <cell r="T15">
-            <v>6000</v>
-          </cell>
-          <cell r="U15">
-            <v>24500</v>
-          </cell>
-          <cell r="V15">
-            <v>30500</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="S16">
-            <v>35</v>
-          </cell>
-          <cell r="T16">
-            <v>6000</v>
-          </cell>
-          <cell r="U16">
-            <v>24500</v>
-          </cell>
-          <cell r="V16">
-            <v>30500</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="S17">
-            <v>36</v>
-          </cell>
-          <cell r="T17">
-            <v>6000</v>
-          </cell>
-          <cell r="U17">
-            <v>24500</v>
-          </cell>
-          <cell r="V17">
-            <v>30500</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1722,7 +1531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F517E49F-3167-EC43-A232-0380675D9406}">
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -1755,14 +1564,14 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
       <c r="T3" t="s">
         <v>2</v>
       </c>
@@ -1781,51 +1590,51 @@
         <v>6</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="5" t="s">
+      <c r="K4" s="5"/>
+      <c r="L4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5" t="s">
+      <c r="R4" s="4"/>
+      <c r="S4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="T4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="U4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1833,20 +1642,20 @@
       <c r="A5" s="1">
         <v>24</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>45452</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>45458</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="6"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="5"/>
       <c r="L5">
         <f>E5</f>
         <v>0</v>
@@ -1890,20 +1699,20 @@
       <c r="A6" s="1">
         <v>25</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>45459</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>45465</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="6"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="5"/>
       <c r="L6">
         <f t="shared" ref="L6:Q17" si="1">L5+E6</f>
         <v>0</v>
@@ -1947,10 +1756,10 @@
       <c r="A7">
         <v>26</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>45466</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>45472</v>
       </c>
       <c r="E7" s="2"/>
@@ -2004,18 +1813,18 @@
       <c r="A8">
         <v>27</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>45473</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>45479</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>2000</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="L8">
@@ -2063,18 +1872,18 @@
       <c r="A9">
         <v>28</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>45480</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>45486</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>5000</v>
       </c>
-      <c r="H9" s="9"/>
+      <c r="H9" s="8"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="L9">
@@ -2122,10 +1931,10 @@
       <c r="A10">
         <v>29</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>45487</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>45493</v>
       </c>
       <c r="E10" s="2">
@@ -2134,10 +1943,10 @@
       <c r="F10" s="2">
         <v>100</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>5000</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="L10">
@@ -2185,10 +1994,10 @@
       <c r="A11">
         <v>30</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>45494</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>45500</v>
       </c>
       <c r="E11" s="2">
@@ -2248,10 +2057,10 @@
       <c r="A12">
         <v>31</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>45501</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>45507</v>
       </c>
       <c r="E12" s="2">
@@ -2313,10 +2122,10 @@
       <c r="A13">
         <v>32</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>45508</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>45514</v>
       </c>
       <c r="E13" s="2"/>
@@ -2370,10 +2179,10 @@
       <c r="A14">
         <v>33</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>45515</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>45521</v>
       </c>
       <c r="E14" s="2"/>
@@ -2427,10 +2236,10 @@
       <c r="A15">
         <v>34</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>45522</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>45528</v>
       </c>
       <c r="E15" s="2"/>
@@ -2484,10 +2293,10 @@
       <c r="A16">
         <v>35</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>45529</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>45535</v>
       </c>
       <c r="E16" s="2"/>
@@ -2541,10 +2350,10 @@
       <c r="A17">
         <v>36</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>45536</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>45542</v>
       </c>
       <c r="E17" s="2"/>
@@ -2595,7 +2404,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="2">
@@ -2645,1111 +2454,1111 @@
       <c r="A1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="12">
+      <c r="A2" s="11">
         <v>45452</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="10">
         <f>VLOOKUP(A2,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>24</v>
       </c>
-      <c r="C2" s="11">
-        <f>VLOOKUP(B2,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C2" s="10" t="e">
+        <f>VLOOKUP(B2,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="12">
+      <c r="A3" s="11">
         <v>45453</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <f>VLOOKUP(A3,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>24</v>
       </c>
-      <c r="C3" s="11">
-        <f>VLOOKUP(B3,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C3" s="10" t="e">
+        <f>VLOOKUP(B3,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="12">
+      <c r="A4" s="11">
         <v>45454</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <f>VLOOKUP(A4,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>24</v>
       </c>
-      <c r="C4" s="11">
-        <f>VLOOKUP(B4,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C4" s="10" t="e">
+        <f>VLOOKUP(B4,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>45455</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <f>VLOOKUP(A5,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>24</v>
       </c>
-      <c r="C5" s="11">
-        <f>VLOOKUP(B5,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C5" s="10" t="e">
+        <f>VLOOKUP(B5,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
+      <c r="A6" s="11">
         <v>45456</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <f>VLOOKUP(A6,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>24</v>
       </c>
-      <c r="C6" s="11">
-        <f>VLOOKUP(B6,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C6" s="10" t="e">
+        <f>VLOOKUP(B6,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
+      <c r="A7" s="11">
         <v>45457</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <f>VLOOKUP(A7,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>24</v>
       </c>
-      <c r="C7" s="11">
-        <f>VLOOKUP(B7,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C7" s="10" t="e">
+        <f>VLOOKUP(B7,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="12">
+      <c r="A8" s="11">
         <v>45458</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <f>VLOOKUP(A8,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>24</v>
       </c>
-      <c r="C8" s="11">
-        <f>VLOOKUP(B8,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C8" s="10" t="e">
+        <f>VLOOKUP(B8,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="12">
+      <c r="A9" s="11">
         <v>45459</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <f>VLOOKUP(A9,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>25</v>
       </c>
-      <c r="C9" s="11">
-        <f>VLOOKUP(B9,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C9" s="10" t="e">
+        <f>VLOOKUP(B9,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="12">
+      <c r="A10" s="11">
         <v>45460</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <f>VLOOKUP(A10,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>25</v>
       </c>
-      <c r="C10" s="11">
-        <f>VLOOKUP(B10,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C10" s="10" t="e">
+        <f>VLOOKUP(B10,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="12">
+      <c r="A11" s="11">
         <v>45461</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <f>VLOOKUP(A11,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>25</v>
       </c>
-      <c r="C11" s="11">
-        <f>VLOOKUP(B11,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C11" s="10" t="e">
+        <f>VLOOKUP(B11,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="12">
+      <c r="A12" s="11">
         <v>45462</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <f>VLOOKUP(A12,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>25</v>
       </c>
-      <c r="C12" s="11">
-        <f>VLOOKUP(B12,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C12" s="10" t="e">
+        <f>VLOOKUP(B12,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="12">
+      <c r="A13" s="11">
         <v>45463</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <f>VLOOKUP(A13,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>25</v>
       </c>
-      <c r="C13" s="11">
-        <f>VLOOKUP(B13,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C13" s="10" t="e">
+        <f>VLOOKUP(B13,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="12">
+      <c r="A14" s="11">
         <v>45464</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <f>VLOOKUP(A14,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>25</v>
       </c>
-      <c r="C14" s="11">
-        <f>VLOOKUP(B14,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C14" s="10" t="e">
+        <f>VLOOKUP(B14,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="12">
+      <c r="A15" s="11">
         <v>45465</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <f>VLOOKUP(A15,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>25</v>
       </c>
-      <c r="C15" s="11">
-        <f>VLOOKUP(B15,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C15" s="10" t="e">
+        <f>VLOOKUP(B15,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="12">
+      <c r="A16" s="11">
         <v>45466</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <f>VLOOKUP(A16,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>26</v>
       </c>
-      <c r="C16" s="11">
-        <f>VLOOKUP(B16,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C16" s="10" t="e">
+        <f>VLOOKUP(B16,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="12">
+      <c r="A17" s="11">
         <v>45467</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <f>VLOOKUP(A17,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>26</v>
       </c>
-      <c r="C17" s="11">
-        <f>VLOOKUP(B17,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C17" s="10" t="e">
+        <f>VLOOKUP(B17,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="12">
+      <c r="A18" s="11">
         <v>45468</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <f>VLOOKUP(A18,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>26</v>
       </c>
-      <c r="C18" s="11">
-        <f>VLOOKUP(B18,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C18" s="10" t="e">
+        <f>VLOOKUP(B18,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="12">
+      <c r="A19" s="11">
         <v>45469</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="10">
         <f>VLOOKUP(A19,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>26</v>
       </c>
-      <c r="C19" s="11">
-        <f>VLOOKUP(B19,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C19" s="10" t="e">
+        <f>VLOOKUP(B19,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="12">
+      <c r="A20" s="11">
         <v>45470</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="10">
         <f>VLOOKUP(A20,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>26</v>
       </c>
-      <c r="C20" s="11">
-        <f>VLOOKUP(B20,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C20" s="10" t="e">
+        <f>VLOOKUP(B20,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="12">
+      <c r="A21" s="11">
         <v>45471</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="10">
         <f>VLOOKUP(A21,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>26</v>
       </c>
-      <c r="C21" s="11">
-        <f>VLOOKUP(B21,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C21" s="10" t="e">
+        <f>VLOOKUP(B21,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="12">
+      <c r="A22" s="11">
         <v>45472</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="10">
         <f>VLOOKUP(A22,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>26</v>
       </c>
-      <c r="C22" s="11">
-        <f>VLOOKUP(B22,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C22" s="10" t="e">
+        <f>VLOOKUP(B22,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="12">
+      <c r="A23" s="11">
         <v>45473</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="10">
         <f>VLOOKUP(A23,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>27</v>
       </c>
-      <c r="C23" s="11">
-        <f>VLOOKUP(B23,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C23" s="10" t="e">
+        <f>VLOOKUP(B23,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="12">
+      <c r="A24" s="11">
         <v>45474</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="10">
         <f>VLOOKUP(A24,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>27</v>
       </c>
-      <c r="C24" s="11">
-        <f>VLOOKUP(B24,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C24" s="10" t="e">
+        <f>VLOOKUP(B24,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="12">
+      <c r="A25" s="11">
         <v>45475</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <f>VLOOKUP(A25,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>27</v>
       </c>
-      <c r="C25" s="11">
-        <f>VLOOKUP(B25,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C25" s="10" t="e">
+        <f>VLOOKUP(B25,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="12">
+      <c r="A26" s="11">
         <v>45476</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="10">
         <f>VLOOKUP(A26,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>27</v>
       </c>
-      <c r="C26" s="11">
-        <f>VLOOKUP(B26,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C26" s="10" t="e">
+        <f>VLOOKUP(B26,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="12">
+      <c r="A27" s="11">
         <v>45477</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="10">
         <f>VLOOKUP(A27,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>27</v>
       </c>
-      <c r="C27" s="11">
-        <f>VLOOKUP(B27,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C27" s="10" t="e">
+        <f>VLOOKUP(B27,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="12">
+      <c r="A28" s="11">
         <v>45478</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="10">
         <f>VLOOKUP(A28,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>27</v>
       </c>
-      <c r="C28" s="11">
-        <f>VLOOKUP(B28,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C28" s="10" t="e">
+        <f>VLOOKUP(B28,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="12">
+      <c r="A29" s="11">
         <v>45479</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B29" s="10">
         <f>VLOOKUP(A29,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>27</v>
       </c>
-      <c r="C29" s="11">
-        <f>VLOOKUP(B29,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>0</v>
+      <c r="C29" s="10" t="e">
+        <f>VLOOKUP(B29,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="12">
+      <c r="A30" s="11">
         <v>45480</v>
       </c>
-      <c r="B30" s="11">
+      <c r="B30" s="10">
         <f>VLOOKUP(A30,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>28</v>
       </c>
-      <c r="C30" s="11">
-        <f>VLOOKUP(B30,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2000</v>
+      <c r="C30" s="10" t="e">
+        <f>VLOOKUP(B30,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="12">
+      <c r="A31" s="11">
         <v>45481</v>
       </c>
-      <c r="B31" s="11">
+      <c r="B31" s="10">
         <f>VLOOKUP(A31,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>28</v>
       </c>
-      <c r="C31" s="11">
-        <f>VLOOKUP(B31,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2000</v>
+      <c r="C31" s="10" t="e">
+        <f>VLOOKUP(B31,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="12">
+      <c r="A32" s="11">
         <v>45482</v>
       </c>
-      <c r="B32" s="11">
+      <c r="B32" s="10">
         <f>VLOOKUP(A32,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>28</v>
       </c>
-      <c r="C32" s="11">
-        <f>VLOOKUP(B32,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2000</v>
+      <c r="C32" s="10" t="e">
+        <f>VLOOKUP(B32,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="12">
+      <c r="A33" s="11">
         <v>45483</v>
       </c>
-      <c r="B33" s="11">
+      <c r="B33" s="10">
         <f>VLOOKUP(A33,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>28</v>
       </c>
-      <c r="C33" s="11">
-        <f>VLOOKUP(B33,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2000</v>
+      <c r="C33" s="10" t="e">
+        <f>VLOOKUP(B33,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="12">
+      <c r="A34" s="11">
         <v>45484</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B34" s="10">
         <f>VLOOKUP(A34,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>28</v>
       </c>
-      <c r="C34" s="11">
-        <f>VLOOKUP(B34,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2000</v>
+      <c r="C34" s="10" t="e">
+        <f>VLOOKUP(B34,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="12">
+      <c r="A35" s="11">
         <v>45485</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B35" s="10">
         <f>VLOOKUP(A35,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>28</v>
       </c>
-      <c r="C35" s="11">
-        <f>VLOOKUP(B35,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2000</v>
+      <c r="C35" s="10" t="e">
+        <f>VLOOKUP(B35,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="12">
+      <c r="A36" s="11">
         <v>45486</v>
       </c>
-      <c r="B36" s="11">
+      <c r="B36" s="10">
         <f>VLOOKUP(A36,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>28</v>
       </c>
-      <c r="C36" s="11">
-        <f>VLOOKUP(B36,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>2000</v>
+      <c r="C36" s="10" t="e">
+        <f>VLOOKUP(B36,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="12">
+      <c r="A37" s="11">
         <v>45487</v>
       </c>
-      <c r="B37" s="11">
+      <c r="B37" s="10">
         <f>VLOOKUP(A37,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>29</v>
       </c>
-      <c r="C37" s="11">
-        <f>VLOOKUP(B37,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7000</v>
+      <c r="C37" s="10" t="e">
+        <f>VLOOKUP(B37,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="12">
+      <c r="A38" s="11">
         <v>45488</v>
       </c>
-      <c r="B38" s="11">
+      <c r="B38" s="10">
         <f>VLOOKUP(A38,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>29</v>
       </c>
-      <c r="C38" s="11">
-        <f>VLOOKUP(B38,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7000</v>
+      <c r="C38" s="10" t="e">
+        <f>VLOOKUP(B38,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="12">
+      <c r="A39" s="11">
         <v>45489</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39" s="10">
         <f>VLOOKUP(A39,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>29</v>
       </c>
-      <c r="C39" s="11">
-        <f>VLOOKUP(B39,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7000</v>
+      <c r="C39" s="10" t="e">
+        <f>VLOOKUP(B39,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="12">
+      <c r="A40" s="11">
         <v>45490</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B40" s="10">
         <f>VLOOKUP(A40,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>29</v>
       </c>
-      <c r="C40" s="11">
-        <f>VLOOKUP(B40,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7000</v>
+      <c r="C40" s="10" t="e">
+        <f>VLOOKUP(B40,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="12">
+      <c r="A41" s="11">
         <v>45491</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B41" s="10">
         <f>VLOOKUP(A41,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>29</v>
       </c>
-      <c r="C41" s="11">
-        <f>VLOOKUP(B41,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7000</v>
+      <c r="C41" s="10" t="e">
+        <f>VLOOKUP(B41,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="12">
+      <c r="A42" s="11">
         <v>45492</v>
       </c>
-      <c r="B42" s="11">
+      <c r="B42" s="10">
         <f>VLOOKUP(A42,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>29</v>
       </c>
-      <c r="C42" s="11">
-        <f>VLOOKUP(B42,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7000</v>
+      <c r="C42" s="10" t="e">
+        <f>VLOOKUP(B42,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="12">
+      <c r="A43" s="11">
         <v>45493</v>
       </c>
-      <c r="B43" s="11">
+      <c r="B43" s="10">
         <f>VLOOKUP(A43,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>29</v>
       </c>
-      <c r="C43" s="11">
-        <f>VLOOKUP(B43,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>7000</v>
+      <c r="C43" s="10" t="e">
+        <f>VLOOKUP(B43,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="12">
+      <c r="A44" s="11">
         <v>45494</v>
       </c>
-      <c r="B44" s="11">
+      <c r="B44" s="10">
         <f>VLOOKUP(A44,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="C44" s="11">
-        <f>VLOOKUP(B44,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>12000</v>
+      <c r="C44" s="10" t="e">
+        <f>VLOOKUP(B44,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="12">
+      <c r="A45" s="11">
         <v>45495</v>
       </c>
-      <c r="B45" s="11">
+      <c r="B45" s="10">
         <f>VLOOKUP(A45,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="C45" s="11">
-        <f>VLOOKUP(B45,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>12000</v>
+      <c r="C45" s="10" t="e">
+        <f>VLOOKUP(B45,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="12">
+      <c r="A46" s="11">
         <v>45496</v>
       </c>
-      <c r="B46" s="11">
+      <c r="B46" s="10">
         <f>VLOOKUP(A46,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="C46" s="11">
-        <f>VLOOKUP(B46,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>12000</v>
+      <c r="C46" s="10" t="e">
+        <f>VLOOKUP(B46,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="12">
+      <c r="A47" s="11">
         <v>45497</v>
       </c>
-      <c r="B47" s="11">
+      <c r="B47" s="10">
         <f>VLOOKUP(A47,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="C47" s="11">
-        <f>VLOOKUP(B47,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>12000</v>
+      <c r="C47" s="10" t="e">
+        <f>VLOOKUP(B47,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="12">
+      <c r="A48" s="11">
         <v>45498</v>
       </c>
-      <c r="B48" s="11">
+      <c r="B48" s="10">
         <f>VLOOKUP(A48,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="C48" s="11">
-        <f>VLOOKUP(B48,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>12000</v>
+      <c r="C48" s="10" t="e">
+        <f>VLOOKUP(B48,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="12">
+      <c r="A49" s="11">
         <v>45499</v>
       </c>
-      <c r="B49" s="11">
+      <c r="B49" s="10">
         <f>VLOOKUP(A49,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="C49" s="11">
-        <f>VLOOKUP(B49,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>12000</v>
+      <c r="C49" s="10" t="e">
+        <f>VLOOKUP(B49,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="12">
+      <c r="A50" s="11">
         <v>45500</v>
       </c>
-      <c r="B50" s="11">
+      <c r="B50" s="10">
         <f>VLOOKUP(A50,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="C50" s="11">
-        <f>VLOOKUP(B50,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>12000</v>
+      <c r="C50" s="10" t="e">
+        <f>VLOOKUP(B50,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="12">
+      <c r="A51" s="11">
         <v>45501</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B51" s="10">
         <f>VLOOKUP(A51,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>31</v>
       </c>
-      <c r="C51" s="11">
-        <f>VLOOKUP(B51,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>17200</v>
+      <c r="C51" s="10" t="e">
+        <f>VLOOKUP(B51,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="12">
+      <c r="A52" s="11">
         <v>45502</v>
       </c>
-      <c r="B52" s="11">
+      <c r="B52" s="10">
         <f>VLOOKUP(A52,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>31</v>
       </c>
-      <c r="C52" s="11">
-        <f>VLOOKUP(B52,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>17200</v>
+      <c r="C52" s="10" t="e">
+        <f>VLOOKUP(B52,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="12">
+      <c r="A53" s="11">
         <v>45503</v>
       </c>
-      <c r="B53" s="11">
+      <c r="B53" s="10">
         <f>VLOOKUP(A53,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>31</v>
       </c>
-      <c r="C53" s="11">
-        <f>VLOOKUP(B53,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>17200</v>
+      <c r="C53" s="10" t="e">
+        <f>VLOOKUP(B53,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="12">
+      <c r="A54" s="11">
         <v>45504</v>
       </c>
-      <c r="B54" s="11">
+      <c r="B54" s="10">
         <f>VLOOKUP(A54,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>31</v>
       </c>
-      <c r="C54" s="11">
-        <f>VLOOKUP(B54,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>17200</v>
+      <c r="C54" s="10" t="e">
+        <f>VLOOKUP(B54,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="12">
+      <c r="A55" s="11">
         <v>45505</v>
       </c>
-      <c r="B55" s="11">
+      <c r="B55" s="10">
         <f>VLOOKUP(A55,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>31</v>
       </c>
-      <c r="C55" s="11">
-        <f>VLOOKUP(B55,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>17200</v>
+      <c r="C55" s="10" t="e">
+        <f>VLOOKUP(B55,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="12">
+      <c r="A56" s="11">
         <v>45506</v>
       </c>
-      <c r="B56" s="11">
+      <c r="B56" s="10">
         <f>VLOOKUP(A56,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>31</v>
       </c>
-      <c r="C56" s="11">
-        <f>VLOOKUP(B56,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>17200</v>
+      <c r="C56" s="10" t="e">
+        <f>VLOOKUP(B56,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="12">
+      <c r="A57" s="11">
         <v>45507</v>
       </c>
-      <c r="B57" s="11">
+      <c r="B57" s="10">
         <f>VLOOKUP(A57,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>31</v>
       </c>
-      <c r="C57" s="11">
-        <f>VLOOKUP(B57,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>17200</v>
+      <c r="C57" s="10" t="e">
+        <f>VLOOKUP(B57,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="12">
+      <c r="A58" s="11">
         <v>45508</v>
       </c>
-      <c r="B58" s="11">
+      <c r="B58" s="10">
         <f>VLOOKUP(A58,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="C58" s="11">
-        <f>VLOOKUP(B58,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>26500</v>
+      <c r="C58" s="10" t="e">
+        <f>VLOOKUP(B58,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="12">
+      <c r="A59" s="11">
         <v>45509</v>
       </c>
-      <c r="B59" s="11">
+      <c r="B59" s="10">
         <f>VLOOKUP(A59,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="C59" s="11">
-        <f>VLOOKUP(B59,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>26500</v>
+      <c r="C59" s="10" t="e">
+        <f>VLOOKUP(B59,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="12">
+      <c r="A60" s="11">
         <v>45510</v>
       </c>
-      <c r="B60" s="11">
+      <c r="B60" s="10">
         <f>VLOOKUP(A60,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="C60" s="11">
-        <f>VLOOKUP(B60,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>26500</v>
+      <c r="C60" s="10" t="e">
+        <f>VLOOKUP(B60,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="12">
+      <c r="A61" s="11">
         <v>45511</v>
       </c>
-      <c r="B61" s="11">
+      <c r="B61" s="10">
         <f>VLOOKUP(A61,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="C61" s="11">
-        <f>VLOOKUP(B61,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>26500</v>
+      <c r="C61" s="10" t="e">
+        <f>VLOOKUP(B61,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="12">
+      <c r="A62" s="11">
         <v>45512</v>
       </c>
-      <c r="B62" s="11">
+      <c r="B62" s="10">
         <f>VLOOKUP(A62,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="C62" s="11">
-        <f>VLOOKUP(B62,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>26500</v>
+      <c r="C62" s="10" t="e">
+        <f>VLOOKUP(B62,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="12">
+      <c r="A63" s="11">
         <v>45513</v>
       </c>
-      <c r="B63" s="11">
+      <c r="B63" s="10">
         <f>VLOOKUP(A63,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="C63" s="11">
-        <f>VLOOKUP(B63,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>26500</v>
+      <c r="C63" s="10" t="e">
+        <f>VLOOKUP(B63,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="12">
+      <c r="A64" s="11">
         <v>45514</v>
       </c>
-      <c r="B64" s="11">
+      <c r="B64" s="10">
         <f>VLOOKUP(A64,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="C64" s="11">
-        <f>VLOOKUP(B64,'[1]Sockeye FSC and Demo'!$S$5:$V$17,4,FALSE)</f>
-        <v>26500</v>
+      <c r="C64" s="10" t="e">
+        <f>VLOOKUP(B64,#REF!,4,FALSE)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="12">
+      <c r="A65" s="11">
         <v>45515</v>
       </c>
-      <c r="B65" s="11">
+      <c r="B65" s="10">
         <f>VLOOKUP(A65,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>33</v>
       </c>
-      <c r="C65" s="11"/>
+      <c r="C65" s="10"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="12">
+      <c r="A66" s="11">
         <v>45516</v>
       </c>
-      <c r="B66" s="11">
+      <c r="B66" s="10">
         <f>VLOOKUP(A66,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>33</v>
       </c>
-      <c r="C66" s="11"/>
+      <c r="C66" s="10"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="12">
+      <c r="A67" s="11">
         <v>45517</v>
       </c>
-      <c r="B67" s="11">
+      <c r="B67" s="10">
         <f>VLOOKUP(A67,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>33</v>
       </c>
-      <c r="C67" s="11"/>
+      <c r="C67" s="10"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="12">
+      <c r="A68" s="11">
         <v>45518</v>
       </c>
-      <c r="B68" s="11">
+      <c r="B68" s="10">
         <f>VLOOKUP(A68,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>33</v>
       </c>
-      <c r="C68" s="11"/>
+      <c r="C68" s="10"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="12">
+      <c r="A69" s="11">
         <v>45519</v>
       </c>
-      <c r="B69" s="11">
+      <c r="B69" s="10">
         <f>VLOOKUP(A69,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>33</v>
       </c>
-      <c r="C69" s="11"/>
+      <c r="C69" s="10"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="12">
+      <c r="A70" s="11">
         <v>45520</v>
       </c>
-      <c r="B70" s="11">
+      <c r="B70" s="10">
         <f>VLOOKUP(A70,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>33</v>
       </c>
-      <c r="C70" s="11"/>
+      <c r="C70" s="10"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="12">
+      <c r="A71" s="11">
         <v>45521</v>
       </c>
-      <c r="B71" s="11">
+      <c r="B71" s="10">
         <f>VLOOKUP(A71,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>33</v>
       </c>
-      <c r="C71" s="11"/>
+      <c r="C71" s="10"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="12">
+      <c r="A72" s="11">
         <v>45522</v>
       </c>
-      <c r="B72" s="11">
+      <c r="B72" s="10">
         <f>VLOOKUP(A72,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="C72" s="11"/>
+      <c r="C72" s="10"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="12">
+      <c r="A73" s="11">
         <v>45523</v>
       </c>
-      <c r="B73" s="11">
+      <c r="B73" s="10">
         <f>VLOOKUP(A73,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="C73" s="11"/>
+      <c r="C73" s="10"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="12">
+      <c r="A74" s="11">
         <v>45524</v>
       </c>
-      <c r="B74" s="11">
+      <c r="B74" s="10">
         <f>VLOOKUP(A74,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="C74" s="11"/>
+      <c r="C74" s="10"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="12">
+      <c r="A75" s="11">
         <v>45525</v>
       </c>
-      <c r="B75" s="11">
+      <c r="B75" s="10">
         <f>VLOOKUP(A75,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="C75" s="11"/>
+      <c r="C75" s="10"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="12">
+      <c r="A76" s="11">
         <v>45526</v>
       </c>
-      <c r="B76" s="11">
+      <c r="B76" s="10">
         <f>VLOOKUP(A76,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="C76" s="11"/>
+      <c r="C76" s="10"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="12">
+      <c r="A77" s="11">
         <v>45527</v>
       </c>
-      <c r="B77" s="11">
+      <c r="B77" s="10">
         <f>VLOOKUP(A77,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="C77" s="11"/>
+      <c r="C77" s="10"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="12">
+      <c r="A78" s="11">
         <v>45528</v>
       </c>
-      <c r="B78" s="11">
+      <c r="B78" s="10">
         <f>VLOOKUP(A78,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="C78" s="11"/>
+      <c r="C78" s="10"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="12">
+      <c r="A79" s="11">
         <v>45529</v>
       </c>
-      <c r="B79" s="11">
+      <c r="B79" s="10">
         <f>VLOOKUP(A79,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="C79" s="11"/>
+      <c r="C79" s="10"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="12">
+      <c r="A80" s="11">
         <v>45530</v>
       </c>
-      <c r="B80" s="11">
+      <c r="B80" s="10">
         <f>VLOOKUP(A80,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="C80" s="11"/>
+      <c r="C80" s="10"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="12">
+      <c r="A81" s="11">
         <v>45531</v>
       </c>
-      <c r="B81" s="11">
+      <c r="B81" s="10">
         <f>VLOOKUP(A81,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="C81" s="11"/>
+      <c r="C81" s="10"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="12">
+      <c r="A82" s="11">
         <v>45532</v>
       </c>
-      <c r="B82" s="11">
+      <c r="B82" s="10">
         <f>VLOOKUP(A82,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="C82" s="11"/>
+      <c r="C82" s="10"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="12">
+      <c r="A83" s="11">
         <v>45533</v>
       </c>
-      <c r="B83" s="11">
+      <c r="B83" s="10">
         <f>VLOOKUP(A83,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="C83" s="11"/>
+      <c r="C83" s="10"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="12">
+      <c r="A84" s="11">
         <v>45534</v>
       </c>
-      <c r="B84" s="11">
+      <c r="B84" s="10">
         <f>VLOOKUP(A84,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="C84" s="11"/>
+      <c r="C84" s="10"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="12">
+      <c r="A85" s="11">
         <v>45535</v>
       </c>
-      <c r="B85" s="11">
+      <c r="B85" s="10">
         <f>VLOOKUP(A85,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="C85" s="11"/>
+      <c r="C85" s="10"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="12">
+      <c r="A86" s="11">
         <v>45536</v>
       </c>
-      <c r="B86" s="11">
+      <c r="B86" s="10">
         <f>VLOOKUP(A86,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>36</v>
       </c>
-      <c r="C86" s="11"/>
+      <c r="C86" s="10"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="12">
+      <c r="A87" s="11">
         <v>45537</v>
       </c>
-      <c r="B87" s="11">
+      <c r="B87" s="10">
         <f>VLOOKUP(A87,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>36</v>
       </c>
-      <c r="C87" s="11"/>
+      <c r="C87" s="10"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="12">
+      <c r="A88" s="11">
         <v>45538</v>
       </c>
-      <c r="B88" s="11">
+      <c r="B88" s="10">
         <f>VLOOKUP(A88,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>36</v>
       </c>
-      <c r="C88" s="11"/>
+      <c r="C88" s="10"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="12">
+      <c r="A89" s="11">
         <v>45539</v>
       </c>
-      <c r="B89" s="11">
+      <c r="B89" s="10">
         <f>VLOOKUP(A89,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>36</v>
       </c>
-      <c r="C89" s="11"/>
+      <c r="C89" s="10"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="12">
+      <c r="A90" s="11">
         <v>45540</v>
       </c>
-      <c r="B90" s="11">
+      <c r="B90" s="10">
         <f>VLOOKUP(A90,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>36</v>
       </c>
-      <c r="C90" s="11"/>
+      <c r="C90" s="10"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="12">
+      <c r="A91" s="11">
         <v>45541</v>
       </c>
-      <c r="B91" s="11">
+      <c r="B91" s="10">
         <f>VLOOKUP(A91,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>36</v>
       </c>
-      <c r="C91" s="11"/>
+      <c r="C91" s="10"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="12">
+      <c r="A92" s="11">
         <v>45542</v>
       </c>
-      <c r="B92" s="11">
+      <c r="B92" s="10">
         <f>VLOOKUP(A92,'[1]Stat weeks'!$A$1:$B$119,2,FALSE)</f>
         <v>36</v>
       </c>
-      <c r="C92" s="11"/>
+      <c r="C92" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3760,8 +3569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A7F00F-86F9-7B42-9119-B394F847541D}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3787,7 +3596,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="12">
+      <c r="A2" s="11">
         <v>45490</v>
       </c>
       <c r="B2" t="s">
@@ -3801,7 +3610,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="12">
+      <c r="A3" s="11">
         <v>45490</v>
       </c>
       <c r="B3" t="s">
@@ -3815,7 +3624,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="12">
+      <c r="A4" s="11">
         <v>45501</v>
       </c>
       <c r="B4" t="s">
@@ -3829,7 +3638,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>45505</v>
       </c>
       <c r="B5" t="s">

</xml_diff>